<commit_message>
Add working Excel file
</commit_message>
<xml_diff>
--- a/BeastSaber-Manager.xlsx
+++ b/BeastSaber-Manager.xlsx
@@ -14,7 +14,119 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+  <si>
+    <t>SongName</t>
+  </si>
+  <si>
+    <t>SongNameURL</t>
+  </si>
+  <si>
+    <t>SongDownloadURL</t>
+  </si>
+  <si>
+    <t>ToDownload</t>
+  </si>
+  <si>
+    <t>Bleed Me Dry – Memphis May Fire</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1ca65/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1ca65</t>
+  </si>
+  <si>
+    <t>Blondie – Rapture (2001 remastered edition)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1cb2e/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1cb2e</t>
+  </si>
+  <si>
+    <t>Calvin Harris – Sweet Nothing (feat. Florence Welch)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1ca5d/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1ca5d</t>
+  </si>
+  <si>
+    <t>Griff – Shade of Yellow</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1cb01/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1cb01</t>
+  </si>
+  <si>
+    <t>I Don’t Like Mondays. – Zenbu Anata no Sei Nan da (It’s All Your Fault)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1c9cc/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1c9cc</t>
+  </si>
+  <si>
+    <t>Minami – DROP</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1ca3f/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1ca3f</t>
+  </si>
+  <si>
+    <t>minato – magnet (Shirayuki Tomoe &amp; Sukoya Kana cover) [Chroma] [#Crossick]</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1ca00/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1ca00</t>
+  </si>
+  <si>
+    <t>New World – Krewella, Yellow Claw ft. Vava</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1c9ac/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1c9ac</t>
+  </si>
+  <si>
+    <t>PBH &amp; Jack – Lose CTRL (feat. Sash Sings)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1c1ed/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1c1ed</t>
+  </si>
+  <si>
+    <t>Redo – Konomi Suzuki</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1c91c/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1c91c</t>
+  </si>
+  <si>
+    <t>Fly Wit Me – Camellia</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1402d/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1402d</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,12 +466,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add refactor to BeastSaber-Manager-Discovery
</commit_message>
<xml_diff>
--- a/BeastSaber-Manager.xlsx
+++ b/BeastSaber-Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1740" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>SongName</t>
   </si>
@@ -28,103 +28,97 @@
     <t>ToDownload</t>
   </si>
   <si>
-    <t>Bleed Me Dry – Memphis May Fire</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1ca65/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1ca65</t>
-  </si>
-  <si>
-    <t>Blondie – Rapture (2001 remastered edition)</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1cb2e/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1cb2e</t>
-  </si>
-  <si>
-    <t>Calvin Harris – Sweet Nothing (feat. Florence Welch)</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1ca5d/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1ca5d</t>
-  </si>
-  <si>
-    <t>Griff – Shade of Yellow</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1cb01/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1cb01</t>
-  </si>
-  <si>
-    <t>I Don’t Like Mondays. – Zenbu Anata no Sei Nan da (It’s All Your Fault)</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1c9cc/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1c9cc</t>
-  </si>
-  <si>
-    <t>Minami – DROP</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1ca3f/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1ca3f</t>
-  </si>
-  <si>
-    <t>minato – magnet (Shirayuki Tomoe &amp; Sukoya Kana cover) [Chroma] [#Crossick]</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1ca00/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1ca00</t>
-  </si>
-  <si>
-    <t>New World – Krewella, Yellow Claw ft. Vava</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1c9ac/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1c9ac</t>
-  </si>
-  <si>
-    <t>PBH &amp; Jack – Lose CTRL (feat. Sash Sings)</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1c1ed/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1c1ed</t>
-  </si>
-  <si>
-    <t>Redo – Konomi Suzuki</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1c91c/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1c91c</t>
-  </si>
-  <si>
-    <t>Fly Wit Me – Camellia</t>
-  </si>
-  <si>
-    <t>https://bsaber.com/songs/1402d/</t>
-  </si>
-  <si>
-    <t>https://api.beatsaver.com/download/key/1402d</t>
+    <t>Daddy – PSY</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/133b/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/133b</t>
+  </si>
+  <si>
+    <t>Imagine Dragons – Believer (100k ver.) | 100k Contest</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/1fef/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/1fef</t>
+  </si>
+  <si>
+    <t>Kero Kero Bonito – Flamingo</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/4e6f/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/4e6f</t>
+  </si>
+  <si>
+    <t>League of Legends – Legends never die (ft. Against The Current)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/66e6/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/66e6</t>
+  </si>
+  <si>
+    <t>Mr. Blue Sky – Electric Light Orchestra</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/570/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/570</t>
+  </si>
+  <si>
+    <t>Muse – Uprising</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/4c6/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/4c6</t>
+  </si>
+  <si>
+    <t>Panic at the disco – The Greatest Showman reimagined | (100K Contest)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/2087/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/2087</t>
+  </si>
+  <si>
+    <t>Shut Up and Dance – WALK THE MOON</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/2144/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/2144</t>
+  </si>
+  <si>
+    <t>Skillet – Feel Invincible</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/121f/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/121f</t>
+  </si>
+  <si>
+    <t>Technologic – Daft Punk (Update)</t>
+  </si>
+  <si>
+    <t>https://bsaber.com/songs/747/</t>
+  </si>
+  <si>
+    <t>https://api.beatsaver.com/download/key/747</t>
+  </si>
+  <si>
+    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -466,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,16 +498,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,27 +526,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -560,55 +554,55 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -616,27 +610,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -644,16 +638,128 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="b">
-        <v>0</v>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2021-10-01 Full List file
</commit_message>
<xml_diff>
--- a/BeastSaber-Manager.xlsx
+++ b/BeastSaber-Manager.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>SongName</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>https://api.beatsaver.com/download/key/747</t>
-  </si>
-  <si>
-    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -460,11 +457,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -506,8 +501,8 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>34</v>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,8 +529,8 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>34</v>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,8 +557,8 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
+      <c r="D7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,19 +585,19 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>34</v>
+      <c r="D9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -618,19 +613,19 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>34</v>
+      <c r="D11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -646,19 +641,19 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>34</v>
+      <c r="D13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -674,19 +669,19 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
-        <v>34</v>
+      <c r="D15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -702,19 +697,19 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
-        <v>34</v>
+      <c r="D17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -730,19 +725,19 @@
       <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s">
-        <v>34</v>
+      <c r="D19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -758,8 +753,22 @@
       <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
-        <v>34</v>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>